<commit_message>
Update 固有名詞 (Literally everything else).xlsx
</commit_message>
<xml_diff>
--- a/English translation/その他文字 (Items, Skills, Characters, Descriptions)/固有名詞 (Literally everything else).xlsx
+++ b/English translation/その他文字 (Items, Skills, Characters, Descriptions)/固有名詞 (Literally everything else).xlsx
@@ -9,7 +9,7 @@
     </mc:Choice>
   </mc:AlternateContent>
   <bookViews>
-    <workbookView xWindow="0" yWindow="0" windowWidth="21943" windowHeight="8091" tabRatio="627" firstSheet="10" activeTab="19"/>
+    <workbookView xWindow="0" yWindow="0" windowWidth="21943" windowHeight="8091" tabRatio="627" firstSheet="5" activeTab="5"/>
   </bookViews>
   <sheets>
     <sheet name="名前" sheetId="1" r:id="rId1"/>
@@ -41,7 +41,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="3640" uniqueCount="2342">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="3640" uniqueCount="2345">
   <si>
     <t>カテゴリ</t>
   </si>
@@ -10893,14 +10893,23 @@
     <t>A bra bellonging to a succubus.</t>
   </si>
   <si>
-    <t>A bra bellonging to a succubus.It smells sweet.</t>
-  </si>
-  <si>
     <t>情報收集→ミラージュを呼び出す【❤】
 まだは包布はずしままストーリー進行</t>
   </si>
   <si>
     <t>もう一度ミラージュを呼び出す【❤】選だ</t>
+  </si>
+  <si>
+    <t>A bra bellonging to a succubus. It smells sweet.</t>
+  </si>
+  <si>
+    <t>HP+5, Str+1, Mag+3</t>
+  </si>
+  <si>
+    <t>Spirit+1, Spd+8, Mov+1</t>
+  </si>
+  <si>
+    <t>Max HP+10, Mag+4, Luk+2</t>
   </si>
 </sst>
 </file>
@@ -18271,7 +18280,7 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:B3"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
+    <sheetView workbookViewId="0">
       <selection activeCell="D9" sqref="D9"/>
     </sheetView>
   </sheetViews>
@@ -18715,8 +18724,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:G203"/>
   <sheetViews>
-    <sheetView topLeftCell="A46" workbookViewId="0">
-      <selection activeCell="D8" sqref="D8"/>
+    <sheetView tabSelected="1" topLeftCell="B151" workbookViewId="0">
+      <selection activeCell="D165" sqref="D165"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="9" defaultRowHeight="14.15"/>
@@ -22079,7 +22088,7 @@
         <v>2249</v>
       </c>
       <c r="D164" s="30" t="s">
-        <v>758</v>
+        <v>2344</v>
       </c>
       <c r="E164" s="34" t="s">
         <v>759</v>
@@ -22653,7 +22662,7 @@
         <v>2275</v>
       </c>
       <c r="D192" s="30" t="s">
-        <v>2339</v>
+        <v>2341</v>
       </c>
       <c r="E192" s="38" t="s">
         <v>853</v>
@@ -22865,7 +22874,7 @@
         <v>2285</v>
       </c>
       <c r="D202" s="30" t="s">
-        <v>895</v>
+        <v>2342</v>
       </c>
       <c r="E202" s="34" t="s">
         <v>896</v>
@@ -22886,7 +22895,7 @@
         <v>2286</v>
       </c>
       <c r="D203" s="30" t="s">
-        <v>899</v>
+        <v>2343</v>
       </c>
       <c r="E203" s="34" t="s">
         <v>900</v>
@@ -23859,7 +23868,7 @@
         <v>908</v>
       </c>
       <c r="C72" s="44" t="s">
-        <v>2340</v>
+        <v>2339</v>
       </c>
       <c r="D72" s="34" t="s">
         <v>1041</v>
@@ -23883,7 +23892,7 @@
       <c r="A74" s="34"/>
       <c r="B74" s="34"/>
       <c r="C74" s="34" t="s">
-        <v>2341</v>
+        <v>2340</v>
       </c>
       <c r="D74" s="34" t="s">
         <v>1041</v>
@@ -24036,7 +24045,7 @@
         <v>908</v>
       </c>
       <c r="C85" s="44" t="s">
-        <v>2340</v>
+        <v>2339</v>
       </c>
       <c r="D85" s="34" t="s">
         <v>1067</v>
@@ -24092,7 +24101,7 @@
         <v>908</v>
       </c>
       <c r="C89" s="44" t="s">
-        <v>2340</v>
+        <v>2339</v>
       </c>
       <c r="D89" s="34" t="s">
         <v>1077</v>
@@ -24116,7 +24125,7 @@
       <c r="A91" s="34"/>
       <c r="B91" s="34"/>
       <c r="C91" s="34" t="s">
-        <v>2341</v>
+        <v>2340</v>
       </c>
       <c r="D91" s="34" t="s">
         <v>1077</v>

</xml_diff>

<commit_message>
update at devs request
</commit_message>
<xml_diff>
--- a/English translation/その他文字 (Items, Skills, Characters, Descriptions)/固有名詞 (Literally everything else).xlsx
+++ b/English translation/その他文字 (Items, Skills, Characters, Descriptions)/固有名詞 (Literally everything else).xlsx
@@ -8295,9 +8295,6 @@
     <t>A junior school girl. Quite cheeky</t>
   </si>
   <si>
-    <t>A junior school girl. Has recently fallen in love.</t>
-  </si>
-  <si>
     <t>A highschool girl with impressive technique and abilities.</t>
   </si>
   <si>
@@ -8347,6 +8344,9 @@
   </si>
   <si>
     <t>An elf with beautiful legs that was converted into a succubus.</t>
+  </si>
+  <si>
+    <t>A junior school girl. Enjoys the concept of love.</t>
   </si>
 </sst>
 </file>
@@ -9062,8 +9062,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:H77"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="E34" zoomScale="85" zoomScaleNormal="85" workbookViewId="0">
-      <selection activeCell="F58" sqref="F58"/>
+    <sheetView tabSelected="1" topLeftCell="E31" zoomScale="85" zoomScaleNormal="85" workbookViewId="0">
+      <selection activeCell="F40" sqref="F40"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="9" defaultRowHeight="14.15"/>
@@ -9847,7 +9847,7 @@
         <v>2300</v>
       </c>
       <c r="F40" s="24" t="s">
-        <v>2736</v>
+        <v>2753</v>
       </c>
       <c r="G40" s="24" t="s">
         <v>80</v>
@@ -9871,7 +9871,7 @@
         <v>2301</v>
       </c>
       <c r="F41" s="24" t="s">
-        <v>2737</v>
+        <v>2736</v>
       </c>
       <c r="G41" s="24" t="s">
         <v>82</v>
@@ -9895,7 +9895,7 @@
         <v>2302</v>
       </c>
       <c r="F42" s="24" t="s">
-        <v>2738</v>
+        <v>2737</v>
       </c>
       <c r="G42" s="24" t="s">
         <v>84</v>
@@ -9919,7 +9919,7 @@
         <v>2303</v>
       </c>
       <c r="F43" s="24" t="s">
-        <v>2739</v>
+        <v>2738</v>
       </c>
       <c r="G43" s="24" t="s">
         <v>86</v>
@@ -9943,7 +9943,7 @@
         <v>2304</v>
       </c>
       <c r="F44" s="24" t="s">
-        <v>2740</v>
+        <v>2739</v>
       </c>
       <c r="G44" s="24" t="s">
         <v>88</v>
@@ -9967,7 +9967,7 @@
         <v>2305</v>
       </c>
       <c r="F45" s="24" t="s">
-        <v>2741</v>
+        <v>2740</v>
       </c>
       <c r="G45" s="37" t="s">
         <v>90</v>
@@ -9991,7 +9991,7 @@
         <v>2306</v>
       </c>
       <c r="F46" s="24" t="s">
-        <v>2742</v>
+        <v>2741</v>
       </c>
       <c r="G46" s="24" t="s">
         <v>92</v>
@@ -10015,7 +10015,7 @@
         <v>2307</v>
       </c>
       <c r="F47" s="24" t="s">
-        <v>2743</v>
+        <v>2742</v>
       </c>
       <c r="G47" s="24" t="s">
         <v>94</v>
@@ -10039,7 +10039,7 @@
         <v>2308</v>
       </c>
       <c r="F48" s="24" t="s">
-        <v>2744</v>
+        <v>2743</v>
       </c>
       <c r="G48" s="24" t="s">
         <v>96</v>
@@ -10063,7 +10063,7 @@
         <v>2309</v>
       </c>
       <c r="F49" s="24" t="s">
-        <v>2745</v>
+        <v>2744</v>
       </c>
       <c r="G49" s="24" t="s">
         <v>98</v>
@@ -10087,7 +10087,7 @@
         <v>2310</v>
       </c>
       <c r="F50" s="24" t="s">
-        <v>2746</v>
+        <v>2745</v>
       </c>
       <c r="G50" s="24" t="s">
         <v>100</v>
@@ -10111,7 +10111,7 @@
         <v>2311</v>
       </c>
       <c r="F51" s="24" t="s">
-        <v>2747</v>
+        <v>2746</v>
       </c>
       <c r="G51" s="24" t="s">
         <v>102</v>
@@ -10135,7 +10135,7 @@
         <v>2312</v>
       </c>
       <c r="F52" s="24" t="s">
-        <v>2748</v>
+        <v>2747</v>
       </c>
       <c r="G52" s="24" t="s">
         <v>104</v>
@@ -10159,7 +10159,7 @@
         <v>2313</v>
       </c>
       <c r="F53" s="24" t="s">
-        <v>2749</v>
+        <v>2748</v>
       </c>
       <c r="G53" s="24" t="s">
         <v>106</v>
@@ -10183,7 +10183,7 @@
         <v>2314</v>
       </c>
       <c r="F54" s="24" t="s">
-        <v>2750</v>
+        <v>2749</v>
       </c>
       <c r="G54" s="24" t="s">
         <v>109</v>
@@ -10207,7 +10207,7 @@
         <v>1995</v>
       </c>
       <c r="F55" s="24" t="s">
-        <v>2751</v>
+        <v>2750</v>
       </c>
       <c r="G55" s="24" t="s">
         <v>112</v>
@@ -10231,7 +10231,7 @@
         <v>2315</v>
       </c>
       <c r="F56" s="24" t="s">
-        <v>2752</v>
+        <v>2751</v>
       </c>
       <c r="G56" s="24" t="s">
         <v>112</v>
@@ -10255,7 +10255,7 @@
         <v>2316</v>
       </c>
       <c r="F57" s="24" t="s">
-        <v>2753</v>
+        <v>2752</v>
       </c>
       <c r="G57" s="24" t="s">
         <v>114</v>

</xml_diff>